<commit_message>
Created interface class for manager
</commit_message>
<xml_diff>
--- a/app/bin/main/Data/ProjectList.xlsx
+++ b/app/bin/main/Data/ProjectList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Modules\Sem 2\SC 2002\SC2002Assignment\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/422dec7f9d966ce9/Desktop/Java Grp Prj/SC2002Assignment/scr/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA0BF88-AC51-41C8-B2D8-C0205076C8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{7EA0BF88-AC51-41C8-B2D8-C0205076C8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E85C67E-5294-48B5-8FA9-D58531855A15}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9660" yWindow="-12645" windowWidth="19200" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,25 +402,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" customWidth="1"/>
-    <col min="13" max="13" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.36328125" customWidth="1"/>
+    <col min="2" max="2" width="21.7265625" customWidth="1"/>
+    <col min="4" max="4" width="24.08984375" customWidth="1"/>
+    <col min="5" max="5" width="22.54296875" customWidth="1"/>
+    <col min="7" max="7" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.54296875" customWidth="1"/>
+    <col min="13" max="13" width="29.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +461,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>

</xml_diff>